<commit_message>
Added a course graph into swe_page, data in all updates and fixed paths and data
</commit_message>
<xml_diff>
--- a/data/course/resultat_kurs_2020.xlsx
+++ b/data/course/resultat_kurs_2020.xlsx
@@ -1,23 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/said/Documents/github/DataVisualisering_Projekt_YhKollen_G1/data/course/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anton\Documents\GIT\DataVisualisering_Projekt_YhKollen_G1\data\course\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AEFA86C-9F12-6E43-9C65-43F4AAF93658}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53599B3D-7A87-4076-A191-6C0250E8639B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16160" yWindow="500" windowWidth="12640" windowHeight="11060" xr2:uid="{D5A1FCBF-B9C0-40F8-8665-3732FDDAF628}"/>
+    <workbookView xWindow="-90" yWindow="210" windowWidth="28890" windowHeight="5955" xr2:uid="{D5A1FCBF-B9C0-40F8-8665-3732FDDAF628}"/>
   </bookViews>
   <sheets>
-    <sheet name="Lista beviljade utbildningar" sheetId="1" r:id="rId1"/>
+    <sheet name="Lista ansökningar" sheetId="1" r:id="rId1"/>
     <sheet name="Definitioner och förklaringar" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lista beviljade utbildningar'!$A$1:$G$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Lista ansökningar'!$A$1:$G$1</definedName>
     <definedName name="Bedömning">#REF!</definedName>
     <definedName name="Beslut">#REF!</definedName>
     <definedName name="Utb.områden">#REF!</definedName>
@@ -657,13 +657,13 @@
     <t>År</t>
   </si>
   <si>
-    <t xml:space="preserve">Kommun </t>
-  </si>
-  <si>
     <t>2020</t>
   </si>
   <si>
     <t>Antal beviljade platser 1</t>
+  </si>
+  <si>
+    <t>Antal beviljade platser 2</t>
   </si>
 </sst>
 </file>
@@ -843,9 +843,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema Office 2013 – 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 – 2022">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -883,7 +883,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 – 2022">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -989,7 +989,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 – 2022">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1141,19 +1141,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2A5C9BD-4E5C-4650-9BA8-10678C62021C}">
   <dimension ref="A1:H102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:P1048576"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="74.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.28515625" style="11" customWidth="1"/>
+    <col min="2" max="2" width="30.5703125" style="11" customWidth="1"/>
     <col min="3" max="3" width="36" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="19.33203125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.5" style="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.7109375" style="16" customWidth="1"/>
+    <col min="5" max="5" width="22.7109375" style="16" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="11" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.5" style="13"/>
+    <col min="8" max="16384" width="9.42578125" style="13"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1167,7 +1168,7 @@
         <v>182</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="E1" s="14" t="s">
         <v>206</v>
@@ -1176,7 +1177,7 @@
         <v>187</v>
       </c>
       <c r="G1" s="9" t="s">
-        <v>204</v>
+        <v>191</v>
       </c>
       <c r="H1" s="10" t="s">
         <v>203</v>
@@ -1205,7 +1206,7 @@
         <v>9</v>
       </c>
       <c r="H2" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1231,7 +1232,7 @@
         <v>13</v>
       </c>
       <c r="H3" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1257,7 +1258,7 @@
         <v>202</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1283,7 +1284,7 @@
         <v>7</v>
       </c>
       <c r="H5" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1309,7 +1310,7 @@
         <v>21</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1335,7 +1336,7 @@
         <v>202</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1361,7 +1362,7 @@
         <v>21</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1387,7 +1388,7 @@
         <v>9</v>
       </c>
       <c r="H9" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1413,7 +1414,7 @@
         <v>181</v>
       </c>
       <c r="H10" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1439,7 +1440,7 @@
         <v>202</v>
       </c>
       <c r="H11" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1465,7 +1466,7 @@
         <v>30</v>
       </c>
       <c r="H12" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1491,7 +1492,7 @@
         <v>3</v>
       </c>
       <c r="H13" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1517,7 +1518,7 @@
         <v>202</v>
       </c>
       <c r="H14" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1543,7 +1544,7 @@
         <v>11</v>
       </c>
       <c r="H15" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1569,7 +1570,7 @@
         <v>21</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1595,7 +1596,7 @@
         <v>21</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1621,7 +1622,7 @@
         <v>11</v>
       </c>
       <c r="H18" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1647,7 +1648,7 @@
         <v>9</v>
       </c>
       <c r="H19" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1673,7 +1674,7 @@
         <v>7</v>
       </c>
       <c r="H20" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1699,7 +1700,7 @@
         <v>202</v>
       </c>
       <c r="H21" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1725,7 +1726,7 @@
         <v>181</v>
       </c>
       <c r="H22" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1751,7 +1752,7 @@
         <v>9</v>
       </c>
       <c r="H23" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1777,7 +1778,7 @@
         <v>202</v>
       </c>
       <c r="H24" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1803,7 +1804,7 @@
         <v>106</v>
       </c>
       <c r="H25" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1829,7 +1830,7 @@
         <v>202</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1855,7 +1856,7 @@
         <v>11</v>
       </c>
       <c r="H27" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1881,7 +1882,7 @@
         <v>11</v>
       </c>
       <c r="H28" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="29" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1907,7 +1908,7 @@
         <v>9</v>
       </c>
       <c r="H29" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1933,7 +1934,7 @@
         <v>13</v>
       </c>
       <c r="H30" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1959,7 +1960,7 @@
         <v>11</v>
       </c>
       <c r="H31" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -1985,7 +1986,7 @@
         <v>9</v>
       </c>
       <c r="H32" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="33" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2011,7 +2012,7 @@
         <v>11</v>
       </c>
       <c r="H33" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2037,7 +2038,7 @@
         <v>202</v>
       </c>
       <c r="H34" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="35" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2063,7 +2064,7 @@
         <v>25</v>
       </c>
       <c r="H35" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2089,7 +2090,7 @@
         <v>11</v>
       </c>
       <c r="H36" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2115,7 +2116,7 @@
         <v>11</v>
       </c>
       <c r="H37" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="38" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2141,7 +2142,7 @@
         <v>74</v>
       </c>
       <c r="H38" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2167,7 +2168,7 @@
         <v>11</v>
       </c>
       <c r="H39" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2193,7 +2194,7 @@
         <v>202</v>
       </c>
       <c r="H40" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="41" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2219,7 +2220,7 @@
         <v>11</v>
       </c>
       <c r="H41" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="42" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2245,7 +2246,7 @@
         <v>11</v>
       </c>
       <c r="H42" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="43" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2271,7 +2272,7 @@
         <v>202</v>
       </c>
       <c r="H43" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2297,7 +2298,7 @@
         <v>202</v>
       </c>
       <c r="H44" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="45" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2323,7 +2324,7 @@
         <v>202</v>
       </c>
       <c r="H45" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="46" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2349,7 +2350,7 @@
         <v>11</v>
       </c>
       <c r="H46" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="47" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2375,7 +2376,7 @@
         <v>202</v>
       </c>
       <c r="H47" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2401,7 +2402,7 @@
         <v>183</v>
       </c>
       <c r="H48" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="49" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2427,7 +2428,7 @@
         <v>202</v>
       </c>
       <c r="H49" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2453,7 +2454,7 @@
         <v>202</v>
       </c>
       <c r="H50" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="51" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2479,7 +2480,7 @@
         <v>45</v>
       </c>
       <c r="H51" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2505,7 +2506,7 @@
         <v>202</v>
       </c>
       <c r="H52" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="53" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2531,7 +2532,7 @@
         <v>183</v>
       </c>
       <c r="H53" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2557,7 +2558,7 @@
         <v>7</v>
       </c>
       <c r="H54" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2583,7 +2584,7 @@
         <v>202</v>
       </c>
       <c r="H55" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2609,7 +2610,7 @@
         <v>202</v>
       </c>
       <c r="H56" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2635,7 +2636,7 @@
         <v>97</v>
       </c>
       <c r="H57" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2661,7 +2662,7 @@
         <v>202</v>
       </c>
       <c r="H58" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2687,7 +2688,7 @@
         <v>106</v>
       </c>
       <c r="H59" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2713,7 +2714,7 @@
         <v>181</v>
       </c>
       <c r="H60" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2739,7 +2740,7 @@
         <v>79</v>
       </c>
       <c r="H61" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2765,7 +2766,7 @@
         <v>9</v>
       </c>
       <c r="H62" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2791,7 +2792,7 @@
         <v>9</v>
       </c>
       <c r="H63" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2817,7 +2818,7 @@
         <v>11</v>
       </c>
       <c r="H64" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2843,7 +2844,7 @@
         <v>31</v>
       </c>
       <c r="H65" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2869,7 +2870,7 @@
         <v>202</v>
       </c>
       <c r="H66" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2895,7 +2896,7 @@
         <v>11</v>
       </c>
       <c r="H67" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2921,7 +2922,7 @@
         <v>202</v>
       </c>
       <c r="H68" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2947,7 +2948,7 @@
         <v>11</v>
       </c>
       <c r="H69" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2973,7 +2974,7 @@
         <v>11</v>
       </c>
       <c r="H70" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -2999,7 +3000,7 @@
         <v>45</v>
       </c>
       <c r="H71" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3025,7 +3026,7 @@
         <v>30</v>
       </c>
       <c r="H72" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3051,7 +3052,7 @@
         <v>45</v>
       </c>
       <c r="H73" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3077,7 +3078,7 @@
         <v>120</v>
       </c>
       <c r="H74" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3103,7 +3104,7 @@
         <v>202</v>
       </c>
       <c r="H75" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3129,7 +3130,7 @@
         <v>11</v>
       </c>
       <c r="H76" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3155,7 +3156,7 @@
         <v>11</v>
       </c>
       <c r="H77" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3181,7 +3182,7 @@
         <v>31</v>
       </c>
       <c r="H78" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3207,7 +3208,7 @@
         <v>3</v>
       </c>
       <c r="H79" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3233,7 +3234,7 @@
         <v>89</v>
       </c>
       <c r="H80" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3259,7 +3260,7 @@
         <v>202</v>
       </c>
       <c r="H81" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3285,7 +3286,7 @@
         <v>160</v>
       </c>
       <c r="H82" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3311,7 +3312,7 @@
         <v>46</v>
       </c>
       <c r="H83" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3337,7 +3338,7 @@
         <v>85</v>
       </c>
       <c r="H84" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3363,7 +3364,7 @@
         <v>92</v>
       </c>
       <c r="H85" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3389,7 +3390,7 @@
         <v>157</v>
       </c>
       <c r="H86" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3415,7 +3416,7 @@
         <v>202</v>
       </c>
       <c r="H87" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3441,7 +3442,7 @@
         <v>168</v>
       </c>
       <c r="H88" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3467,7 +3468,7 @@
         <v>160</v>
       </c>
       <c r="H89" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3493,7 +3494,7 @@
         <v>3</v>
       </c>
       <c r="H90" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3519,7 +3520,7 @@
         <v>3</v>
       </c>
       <c r="H91" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3545,7 +3546,7 @@
         <v>89</v>
       </c>
       <c r="H92" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3571,7 +3572,7 @@
         <v>89</v>
       </c>
       <c r="H93" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3597,7 +3598,7 @@
         <v>157</v>
       </c>
       <c r="H94" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3623,7 +3624,7 @@
         <v>7</v>
       </c>
       <c r="H95" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3649,7 +3650,7 @@
         <v>202</v>
       </c>
       <c r="H96" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3675,7 +3676,7 @@
         <v>46</v>
       </c>
       <c r="H97" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3701,7 +3702,7 @@
         <v>157</v>
       </c>
       <c r="H98" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3727,7 +3728,7 @@
         <v>46</v>
       </c>
       <c r="H99" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3753,7 +3754,7 @@
         <v>202</v>
       </c>
       <c r="H100" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3779,7 +3780,7 @@
         <v>48</v>
       </c>
       <c r="H101" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.2">
@@ -3805,7 +3806,7 @@
         <v>74</v>
       </c>
       <c r="H102" s="13" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
   </sheetData>
@@ -3833,12 +3834,12 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="9.1640625" style="6"/>
+    <col min="1" max="16384" width="9.140625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:71" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:71" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>188</v>
       </c>
@@ -3912,7 +3913,7 @@
       <c r="BR1" s="4"/>
       <c r="BS1" s="4"/>
     </row>
-    <row r="2" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="C2" s="7"/>
       <c r="D2" s="7"/>
@@ -3984,7 +3985,7 @@
       <c r="BR2" s="7"/>
       <c r="BS2" s="7"/>
     </row>
-    <row r="3" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>189</v>
       </c>
@@ -4058,7 +4059,7 @@
       <c r="BR3" s="7"/>
       <c r="BS3" s="7"/>
     </row>
-    <row r="4" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>190</v>
       </c>
@@ -4132,7 +4133,7 @@
       <c r="BR4" s="7"/>
       <c r="BS4" s="7"/>
     </row>
-    <row r="5" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>200</v>
       </c>
@@ -4207,7 +4208,7 @@
       <c r="BS5" s="7"/>
     </row>
     <row r="6" spans="1:71" s="1" customFormat="1" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="7" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>191</v>
       </c>
@@ -4281,7 +4282,7 @@
       <c r="BR7" s="7"/>
       <c r="BS7" s="7"/>
     </row>
-    <row r="8" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>198</v>
       </c>
@@ -4355,7 +4356,7 @@
       <c r="BR8" s="7"/>
       <c r="BS8" s="7"/>
     </row>
-    <row r="9" spans="1:71" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:71" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
       <c r="B9" s="7"/>
       <c r="C9" s="7"/>
@@ -4428,7 +4429,7 @@
       <c r="BR9" s="7"/>
       <c r="BS9" s="7"/>
     </row>
-    <row r="10" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>192</v>
       </c>
@@ -4502,7 +4503,7 @@
       <c r="BR10" s="7"/>
       <c r="BS10" s="7"/>
     </row>
-    <row r="11" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
         <v>201</v>
       </c>
@@ -4576,8 +4577,8 @@
       <c r="BR11" s="7"/>
       <c r="BS11" s="7"/>
     </row>
-    <row r="12" spans="1:71" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="13" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:71" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>193</v>
       </c>
@@ -4651,7 +4652,7 @@
       <c r="BR13" s="7"/>
       <c r="BS13" s="7"/>
     </row>
-    <row r="14" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
         <v>199</v>
       </c>
@@ -4725,7 +4726,7 @@
       <c r="BR14" s="7"/>
       <c r="BS14" s="7"/>
     </row>
-    <row r="15" spans="1:71" ht="6" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:71" ht="6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="5"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -4797,7 +4798,7 @@
       <c r="BR15" s="7"/>
       <c r="BS15" s="7"/>
     </row>
-    <row r="16" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>182</v>
       </c>
@@ -4871,7 +4872,7 @@
       <c r="BR16" s="7"/>
       <c r="BS16" s="7"/>
     </row>
-    <row r="17" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>194</v>
       </c>
@@ -4945,7 +4946,7 @@
       <c r="BR17" s="7"/>
       <c r="BS17" s="7"/>
     </row>
-    <row r="18" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>195</v>
       </c>
@@ -5019,7 +5020,7 @@
       <c r="BR18" s="7"/>
       <c r="BS18" s="7"/>
     </row>
-    <row r="19" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>196</v>
       </c>
@@ -5093,8 +5094,8 @@
       <c r="BR19" s="7"/>
       <c r="BS19" s="7"/>
     </row>
-    <row r="20" spans="1:71" ht="6" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="21" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:71" ht="6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>187</v>
       </c>
@@ -5168,7 +5169,7 @@
       <c r="BR21" s="7"/>
       <c r="BS21" s="7"/>
     </row>
-    <row r="22" spans="1:71" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:71" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
         <v>197</v>
       </c>

</xml_diff>